<commit_message>
Update advice from AI
</commit_message>
<xml_diff>
--- a/knowledge_log.xlsx
+++ b/knowledge_log.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Science</t>
+  </si>
+  <si>
+    <t>2025-08-26 18:02:57</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,6 +182,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>530.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1570.0</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Send email stock knowledge correctly
</commit_message>
<xml_diff>
--- a/knowledge_log.xlsx
+++ b/knowledge_log.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Build Tools</t>
+  </si>
+  <si>
+    <t>2025-09-23 05:00:13</t>
+  </si>
+  <si>
+    <t>Gradle Basics</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -510,6 +516,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>486.0</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>